<commit_message>
cleaned up textgrids for intonation
</commit_message>
<xml_diff>
--- a/VerbConjugation/XLSX/Arm.xlsx
+++ b/VerbConjugation/XLSX/Arm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hovsep/Library/CloudStorage/GoogleDrive-hovsep443@hotmail.com/My Drive/Dialectal kickstarts/2021 kickstart  - Tehran/Archive/iranian_armenian/VerbConjugation/XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A165F-BCB2-AD41-A640-79CBAF00C209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82096DF-2A99-844C-AC2A-804A4C4B92BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="500" windowWidth="28040" windowHeight="15460" xr2:uid="{B2297C89-19AD-CE43-8C13-F47C72A1FD76}"/>
+    <workbookView xWindow="1860" yWindow="1640" windowWidth="28040" windowHeight="15460" xr2:uid="{B2297C89-19AD-CE43-8C13-F47C72A1FD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11731,42 +11731,6 @@
     <t>negative of periphrastic future 3PL</t>
   </si>
   <si>
-    <t>periphrastic future in the past 1SG</t>
-  </si>
-  <si>
-    <t>periphrastic future in the past 2SG</t>
-  </si>
-  <si>
-    <t>periphrastic future in the past 3SG</t>
-  </si>
-  <si>
-    <t>periphrastic future in the past 1PL</t>
-  </si>
-  <si>
-    <t>periphrastic future in the past 2PL</t>
-  </si>
-  <si>
-    <t>periphrastic future in the past 3PL</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 1SG</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 2SG</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 3SG</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 1PL</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 2PL</t>
-  </si>
-  <si>
-    <t>negative of periphrastic future in the past 3PL</t>
-  </si>
-  <si>
     <t>synthetic future 1SG</t>
   </si>
   <si>
@@ -11803,40 +11767,76 @@
     <t>negative of synthetic future 3PL</t>
   </si>
   <si>
-    <t>synthetic future in the past 1SG</t>
-  </si>
-  <si>
-    <t>synthetic future in the past 2SG</t>
-  </si>
-  <si>
-    <t>synthetic future in the past 3SG</t>
-  </si>
-  <si>
-    <t>synthetic future in the past 1PL</t>
-  </si>
-  <si>
-    <t>synthetic future in the past 2PL</t>
-  </si>
-  <si>
-    <t>synthetic future in the past 3PL</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 1SG</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 2SG</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 3SG</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 1PL</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 2PL</t>
-  </si>
-  <si>
-    <t>negative of synthetic future in the past 3PL</t>
+    <t>future in the past 1SG</t>
+  </si>
+  <si>
+    <t>future in the past 2SG</t>
+  </si>
+  <si>
+    <t>future in the past 3SG</t>
+  </si>
+  <si>
+    <t>future in the past 1PL</t>
+  </si>
+  <si>
+    <t>future in the past 2PL</t>
+  </si>
+  <si>
+    <t>future in the past 3PL</t>
+  </si>
+  <si>
+    <t>negative future in the past 1SG</t>
+  </si>
+  <si>
+    <t>negative future in the past 2SG</t>
+  </si>
+  <si>
+    <t>negative future in the past 3SG</t>
+  </si>
+  <si>
+    <t>negative future in the past 1PL</t>
+  </si>
+  <si>
+    <t>negative future in the past 2PL</t>
+  </si>
+  <si>
+    <t>negative future in the past 3PL</t>
+  </si>
+  <si>
+    <t>conditional past 1SG</t>
+  </si>
+  <si>
+    <t>conditional past 2SG</t>
+  </si>
+  <si>
+    <t>conditional past 3SG</t>
+  </si>
+  <si>
+    <t>conditional past 1PL</t>
+  </si>
+  <si>
+    <t>conditional past 2PL</t>
+  </si>
+  <si>
+    <t>conditional past 3PL</t>
+  </si>
+  <si>
+    <t>negative conditional past 1SG</t>
+  </si>
+  <si>
+    <t>negative conditional past 2SG</t>
+  </si>
+  <si>
+    <t>negative conditional past 3SG</t>
+  </si>
+  <si>
+    <t>negative conditional past 1PL</t>
+  </si>
+  <si>
+    <t>negative conditional past 2PL</t>
+  </si>
+  <si>
+    <t>negative conditional past 3PL</t>
   </si>
 </sst>
 </file>
@@ -12198,7 +12198,7 @@
   <dimension ref="A1:AD152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129:XFD152"/>
+      <selection activeCell="I142" sqref="I142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22299,7 +22299,7 @@
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>3898</v>
+        <v>3910</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>1308</v>
@@ -22385,7 +22385,7 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>3899</v>
+        <v>3911</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>1334</v>
@@ -22471,7 +22471,7 @@
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>3900</v>
+        <v>3912</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>1360</v>
@@ -22557,7 +22557,7 @@
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>3901</v>
+        <v>3913</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>1386</v>
@@ -22643,7 +22643,7 @@
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>3902</v>
+        <v>3914</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>1412</v>
@@ -22729,7 +22729,7 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>3903</v>
+        <v>3915</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>1438</v>
@@ -22815,7 +22815,7 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>3904</v>
+        <v>3916</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>1464</v>
@@ -22901,7 +22901,7 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>3905</v>
+        <v>3917</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>1490</v>
@@ -22987,7 +22987,7 @@
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>3906</v>
+        <v>3918</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>1516</v>
@@ -23073,7 +23073,7 @@
     </row>
     <row r="126" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>3907</v>
+        <v>3919</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>1542</v>
@@ -23159,7 +23159,7 @@
     </row>
     <row r="127" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>3908</v>
+        <v>3920</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>1568</v>
@@ -23245,7 +23245,7 @@
     </row>
     <row r="128" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>3909</v>
+        <v>3921</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>1594</v>
@@ -23331,7 +23331,7 @@
     </row>
     <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>3910</v>
+        <v>3898</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>2824</v>
@@ -23417,7 +23417,7 @@
     </row>
     <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>3911</v>
+        <v>3899</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>2840</v>
@@ -23503,7 +23503,7 @@
     </row>
     <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>3912</v>
+        <v>3900</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>2856</v>
@@ -23589,7 +23589,7 @@
     </row>
     <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>3913</v>
+        <v>3901</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>2872</v>
@@ -23675,7 +23675,7 @@
     </row>
     <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>3914</v>
+        <v>3902</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>2888</v>
@@ -23761,7 +23761,7 @@
     </row>
     <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>3915</v>
+        <v>3903</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>2904</v>
@@ -23847,7 +23847,7 @@
     </row>
     <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>3916</v>
+        <v>3904</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>2920</v>
@@ -23933,7 +23933,7 @@
     </row>
     <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>3917</v>
+        <v>3905</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>2946</v>
@@ -24019,7 +24019,7 @@
     </row>
     <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>3918</v>
+        <v>3906</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>2972</v>
@@ -24105,7 +24105,7 @@
     </row>
     <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>3919</v>
+        <v>3907</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>2998</v>
@@ -24191,7 +24191,7 @@
     </row>
     <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>3920</v>
+        <v>3908</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>3024</v>
@@ -24277,7 +24277,7 @@
     </row>
     <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>3921</v>
+        <v>3909</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>3050</v>

</xml_diff>